<commit_message>
Quick registration module: Names Field (Done)
</commit_message>
<xml_diff>
--- a/usuarios_registrados.xlsx
+++ b/usuarios_registrados.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ddcre\Desktop\INNOVA\INNOVA WEB\INNOVA AUTOMATION\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25ECC67A-B6C4-4DBC-9DF5-CEE00D7E8038}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="88">
   <si>
     <t>documento</t>
   </si>
@@ -281,13 +275,16 @@
   </si>
   <si>
     <t>66000331test@gmail.com</t>
+  </si>
+  <si>
+    <t>66000093test@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -324,21 +321,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -376,7 +365,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -410,7 +399,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -445,10 +433,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -621,18 +608,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D51"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.5546875" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -646,7 +629,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>66000006</v>
       </c>
@@ -660,7 +643,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -674,7 +657,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -688,7 +671,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -702,7 +685,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -716,7 +699,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -730,7 +713,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -744,7 +727,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -758,7 +741,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -772,7 +755,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -786,7 +769,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -800,7 +783,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -814,7 +797,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -828,7 +811,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -842,7 +825,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -856,7 +839,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -870,7 +853,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>36</v>
       </c>
@@ -884,7 +867,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -898,7 +881,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>40</v>
       </c>
@@ -912,7 +895,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>42</v>
       </c>
@@ -926,7 +909,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>44</v>
       </c>
@@ -940,9 +923,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4">
       <c r="A23">
-        <v>66000034.200000003</v>
+        <v>66000034.2</v>
       </c>
       <c r="B23" t="s">
         <v>46</v>
@@ -954,7 +937,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
         <v>47</v>
       </c>
@@ -968,7 +951,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
         <v>49</v>
       </c>
@@ -982,7 +965,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
         <v>51</v>
       </c>
@@ -996,7 +979,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>53</v>
       </c>
@@ -1010,7 +993,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
         <v>55</v>
       </c>
@@ -1024,7 +1007,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
         <v>57</v>
       </c>
@@ -1038,7 +1021,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4">
       <c r="A30" t="s">
         <v>59</v>
       </c>
@@ -1052,7 +1035,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4">
       <c r="A31" t="s">
         <v>61</v>
       </c>
@@ -1066,7 +1049,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4">
       <c r="A32">
         <v>66000001</v>
       </c>
@@ -1080,7 +1063,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4">
       <c r="A33">
         <v>660000000000049</v>
       </c>
@@ -1094,7 +1077,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4">
       <c r="A34">
         <v>6650</v>
       </c>
@@ -1108,7 +1091,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4">
       <c r="A35">
         <v>66000051</v>
       </c>
@@ -1122,7 +1105,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4">
       <c r="A36">
         <v>66000052</v>
       </c>
@@ -1136,7 +1119,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4">
       <c r="A37">
         <v>66000053</v>
       </c>
@@ -1150,7 +1133,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4">
       <c r="A38">
         <v>76000053</v>
       </c>
@@ -1164,7 +1147,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4">
       <c r="A39">
         <v>77000053</v>
       </c>
@@ -1178,7 +1161,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4">
       <c r="A40">
         <v>66000054</v>
       </c>
@@ -1192,7 +1175,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4">
       <c r="A41">
         <v>66000054</v>
       </c>
@@ -1206,7 +1189,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4">
       <c r="A42">
         <v>76000054</v>
       </c>
@@ -1220,7 +1203,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4">
       <c r="A43">
         <v>76000054</v>
       </c>
@@ -1234,7 +1217,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4">
       <c r="A44">
         <v>72000054</v>
       </c>
@@ -1248,7 +1231,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4">
       <c r="A45">
         <v>72000054</v>
       </c>
@@ -1262,7 +1245,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4">
       <c r="A46">
         <v>73000054</v>
       </c>
@@ -1276,7 +1259,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4">
       <c r="A47">
         <v>73000054</v>
       </c>
@@ -1290,7 +1273,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4">
       <c r="A48" t="s">
         <v>79</v>
       </c>
@@ -1304,7 +1287,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4">
       <c r="A49" t="s">
         <v>81</v>
       </c>
@@ -1318,7 +1301,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4">
       <c r="A50" t="s">
         <v>83</v>
       </c>
@@ -1332,7 +1315,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4">
       <c r="A51" t="s">
         <v>85</v>
       </c>
@@ -1343,6 +1326,20 @@
         <v>66000331</v>
       </c>
       <c r="D51" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52">
+        <v>66000093</v>
+      </c>
+      <c r="B52" t="s">
+        <v>87</v>
+      </c>
+      <c r="C52">
+        <v>66000093</v>
+      </c>
+      <c r="D52" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Quick registration module: First Surname Field (Done)
</commit_message>
<xml_diff>
--- a/usuarios_registrados.xlsx
+++ b/usuarios_registrados.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="90">
   <si>
     <t>documento</t>
   </si>
@@ -278,6 +278,12 @@
   </si>
   <si>
     <t>66000093test@gmail.com</t>
+  </si>
+  <si>
+    <t>66000128test@gmail.com</t>
+  </si>
+  <si>
+    <t>66000129test@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -609,7 +615,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:D54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1343,6 +1349,34 @@
         <v>5</v>
       </c>
     </row>
+    <row r="53" spans="1:4">
+      <c r="A53">
+        <v>66000128</v>
+      </c>
+      <c r="B53" t="s">
+        <v>88</v>
+      </c>
+      <c r="C53">
+        <v>66000128</v>
+      </c>
+      <c r="D53" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54">
+        <v>66000129</v>
+      </c>
+      <c r="B54" t="s">
+        <v>89</v>
+      </c>
+      <c r="C54">
+        <v>66000129</v>
+      </c>
+      <c r="D54" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>